<commit_message>
Next Manual cleaning of data
</commit_message>
<xml_diff>
--- a/Data Collection/Authors/Katja Gentinetta/Gentinetta_all_2021.xlsx
+++ b/Data Collection/Authors/Katja Gentinetta/Gentinetta_all_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c6ad9d82f21af58/Dokumente/COINS_SwissTribeleaders/Data Collection/Authors/Katja Gentinetta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12DE2BD9-6975-474C-BB62-C66F783722E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{12DE2BD9-6975-474C-BB62-C66F783722E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E1864FE-1929-4190-AE65-F6D8F180138F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,7 +458,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -543,10 +543,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,6 +945,9 @@
       <c r="G2" t="s">
         <v>17</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -967,6 +970,9 @@
       </c>
       <c r="G3" t="s">
         <v>18</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -991,6 +997,9 @@
       <c r="G4" t="s">
         <v>19</v>
       </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1008,11 +1017,14 @@
       <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1031,11 +1043,14 @@
       <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>28</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1054,11 +1069,14 @@
       <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>32</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1077,11 +1095,14 @@
       <c r="E8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>37</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1100,11 +1121,14 @@
       <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1123,11 +1147,14 @@
       <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>45</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1146,11 +1173,14 @@
       <c r="E11" t="s">
         <v>48</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>50</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1169,11 +1199,14 @@
       <c r="E12" t="s">
         <v>52</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>53</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1192,11 +1225,14 @@
       <c r="E13" t="s">
         <v>57</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>58</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>59</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1215,11 +1251,14 @@
       <c r="E14" t="s">
         <v>61</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>62</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>63</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1238,11 +1277,14 @@
       <c r="E15" t="s">
         <v>65</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>67</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1261,14 +1303,17 @@
       <c r="E16" t="s">
         <v>69</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>70</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1284,14 +1329,17 @@
       <c r="E17" t="s">
         <v>73</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1307,14 +1355,17 @@
       <c r="E18" t="s">
         <v>78</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>79</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1330,14 +1381,17 @@
       <c r="E19" t="s">
         <v>82</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>83</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1353,14 +1407,17 @@
       <c r="E20" t="s">
         <v>87</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1376,14 +1433,17 @@
       <c r="E21" t="s">
         <v>91</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>92</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1399,14 +1459,17 @@
       <c r="E22" t="s">
         <v>96</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>97</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1422,14 +1485,17 @@
       <c r="E23" t="s">
         <v>100</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>101</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1445,14 +1511,17 @@
       <c r="E24" t="s">
         <v>104</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>105</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1468,11 +1537,14 @@
       <c r="E25" t="s">
         <v>108</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>109</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>110</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1480,8 +1552,29 @@
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{7A088B32-9444-4F38-90DD-DD749F0E9D02}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{9D4F2294-E3E6-4ED6-A7C0-1BBE721E1B7B}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{F510A422-C9A9-4B3D-AAC5-18B14D642916}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{974938AA-FAE8-4B53-9576-6772C318585C}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{FE5CD5AB-DBF7-41E4-A831-216DA0264690}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{C5891E4B-ADA5-4BFC-AFCF-B70D696D7A7D}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{0DC263AE-CEF7-480D-9810-2AECD1179757}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{AF9CAEEA-16D9-47B4-9BC5-AE29F7DFCE07}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{8BEC7F7B-F91F-47BF-87D8-ED84E7794307}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{DD1F77C7-CEDF-43AE-A1CE-8D308FDE2CD6}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{6EA9EB29-EC93-4EB6-A755-A663BE239A55}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{58914B58-BA31-4422-9B41-7C894EDB98DA}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{BABB381E-59DD-4C2C-BD87-91E36340E1F7}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{9D484BF9-C4D0-40A2-A50B-66F4053CE5E2}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{AAA75287-97C7-4153-81AC-8C465996DCF8}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{8F2ADD10-1BD0-4335-B7FD-3466AE105DA9}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{F98ACFA1-74A8-4122-B01E-0E32313389B2}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{64C9115D-80DA-4296-90CD-56A206D85671}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{A43403CD-0DF8-4221-845A-EF0E34708FBC}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{91C4E47E-3D1C-4003-800A-52F082F825AB}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{CFD28FCC-8085-4816-BAEB-DA6048B8B173}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>